<commit_message>
Yichi has added info
</commit_message>
<xml_diff>
--- a/wds_1_timesheet.xlsx
+++ b/wds_1_timesheet.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowWidth="28110" windowHeight="13140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
+  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
+  <si>
+    <t>学习时间 （2016/02/29 - 2016/03/06）</t>
+  </si>
   <si>
     <t>星期一</t>
   </si>
@@ -39,45 +43,105 @@
     <t>星期日</t>
   </si>
   <si>
+    <t>合计</t>
+  </si>
+  <si>
     <t>张宏</t>
   </si>
   <si>
     <t>张怡弛</t>
   </si>
   <si>
+    <t>张晓冰</t>
+  </si>
+  <si>
     <t>周松</t>
   </si>
   <si>
     <t>周存良</t>
   </si>
   <si>
-    <t>张晓冰</t>
-  </si>
-  <si>
-    <t>合计</t>
-  </si>
-  <si>
-    <t>学习时间 （2016/02/29 - 2016/03/06）</t>
+    <r>
+      <t>学习时间</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2016/03/7 - 2016/03/13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -89,7 +153,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor indexed="47"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -118,12 +182,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -133,10 +195,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -146,34 +210,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="百分比" xfId="4" builtinId="5"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -218,69 +303,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,8 +500,8 @@
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
+                <a:satMod val="350000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
@@ -450,171 +537,355 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="_h" fmla="val 21600"/>
+            <a:gd name="_w" fmla="val 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:pathLst>
+            <a:path w="21600" h="21600"/>
+          </a:pathLst>
+        </a:custGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:srgbClr val="9CBEE0"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="739CC3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="200000"/>
+        </a:ln>
+      </a:spPr>
+      <a:bodyPr/>
+      <a:lstStyle/>
+    </a:spDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="7">
+        <f>SUM(B3:H3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="7">
+        <f t="shared" ref="I4:I7" si="0">SUM(B4:H4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="7">
+        <f>SUM(B5:H5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="7">
+        <f>SUM(B6:H6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="6">
-        <f>SUM(B3:H3 )</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="6">
-        <f t="shared" ref="I4:I7" si="0">SUM(B4:H4 )</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="6">
-        <f t="shared" si="0"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="7">
+        <f>SUM(B7:H7)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
+  <sheetData>
+    <row r="1" customFormat="1" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" spans="1:9">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:9">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I7" si="0">SUM(B3:H3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" spans="1:9">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="7">
+        <f>SUM(B4:H4)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:9">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="7">
+        <f>SUM(B5:H5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" spans="1:9">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="7">
+        <f>SUM(B6:H6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" spans="1:9">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="7">
+        <f>SUM(B7:H7)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Zhang, Yichi add week's study hours of Mar. 14 to Mar. 20
</commit_message>
<xml_diff>
--- a/wds_1_timesheet.xlsx
+++ b/wds_1_timesheet.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28110" windowHeight="13140" activeTab="1"/>
+    <workbookView windowWidth="28695" windowHeight="13155" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="2.29-3.06" sheetId="1" r:id="rId1"/>
+    <sheet name="3.7-3.13" sheetId="2" r:id="rId2"/>
+    <sheet name="3.14-3.20" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
   <si>
     <t>学习时间 （2016/02/29 - 2016/03/06）</t>
   </si>
@@ -62,6 +61,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>学习时间</t>
     </r>
     <r>
@@ -69,7 +74,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -79,7 +83,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>（</t>
@@ -89,7 +92,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>2016/03/7 - 2016/03/13</t>
@@ -99,7 +101,47 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>学习时间</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2016/03/14 - 2016/03/20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>）</t>
@@ -111,40 +153,200 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,8 +359,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -168,69 +556,296 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -245,14 +860,58 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -303,71 +962,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
         <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
         <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -589,7 +1248,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="1:1048576"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
@@ -682,7 +1341,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="5"/>
       <c r="I5" s="7">
-        <f>SUM(B5:H5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -698,7 +1357,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="7">
-        <f>SUM(B6:H6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -714,7 +1373,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="7">
-        <f>SUM(B7:H7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -730,14 +1389,14 @@
   <sheetPr/>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
   <sheetData>
     <row r="1" customFormat="1" spans="2:2">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -810,12 +1469,18 @@
         <v>2</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5">
+        <v>6</v>
+      </c>
       <c r="I4" s="7">
-        <f>SUM(B4:H4)</f>
-        <v>6.5</v>
+        <f t="shared" si="0"/>
+        <v>18.5</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:9">
@@ -830,7 +1495,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="5"/>
       <c r="I5" s="7">
-        <f>SUM(B5:H5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -846,7 +1511,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="7">
-        <f>SUM(B6:H6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -862,7 +1527,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="7">
-        <f>SUM(B7:H7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -876,14 +1541,138 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E22:E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
+  <sheetData>
+    <row r="1" customFormat="1" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" spans="1:9">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:9">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" customFormat="1" spans="1:9">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" ref="I3:I7" si="0">SUM(B4:H4)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:9">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" spans="1:9">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" spans="1:9">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>